<commit_message>
Worked on card ideas & other minor design changes
</commit_message>
<xml_diff>
--- a/doodle-deck-vault/cards.xlsx
+++ b/doodle-deck-vault/cards.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezb12\OneDrive\Desktop\doodle-deck\doodle-deck-vault\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBDC55F-A202-4D6E-8A59-E9AE9E307D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA36B267-47E6-4DB3-87CE-6D8BA124816D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
     <sheet name="Spells &amp; Swift Spells" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Units!$A$1:$E$4</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -44,6 +47,237 @@
   </si>
   <si>
     <t>E-Cost</t>
+  </si>
+  <si>
+    <t>Goblin</t>
+  </si>
+  <si>
+    <t>Kitten</t>
+  </si>
+  <si>
+    <t>Light Footed</t>
+  </si>
+  <si>
+    <t>Golem</t>
+  </si>
+  <si>
+    <t>Reaper</t>
+  </si>
+  <si>
+    <t>Vampiric, Cleave</t>
+  </si>
+  <si>
+    <t>Bat</t>
+  </si>
+  <si>
+    <t>Vampiric</t>
+  </si>
+  <si>
+    <t>Inspiration</t>
+  </si>
+  <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Grand Inspiration</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Give a Unit 3 extra Damage this Round</t>
+  </si>
+  <si>
+    <t>Give a Unit 1 extra Damage this Round</t>
+  </si>
+  <si>
+    <t>Give a Unit an extra Action this Turn</t>
+  </si>
+  <si>
+    <t>Teleport</t>
+  </si>
+  <si>
+    <t>Quick Teleport</t>
+  </si>
+  <si>
+    <t>Swift Spell</t>
+  </si>
+  <si>
+    <t>Move a Unit to a chosen Slot</t>
+  </si>
+  <si>
+    <t>Fireball</t>
+  </si>
+  <si>
+    <t>Dart</t>
+  </si>
+  <si>
+    <t>Deal 1 Damage to a Unit</t>
+  </si>
+  <si>
+    <t>Deal 2 Damage to a Unit</t>
+  </si>
+  <si>
+    <t>Threaten</t>
+  </si>
+  <si>
+    <t>Make a Unit Intimidated</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Bathe</t>
+  </si>
+  <si>
+    <t>Removes all Status Effects from a Unit</t>
+  </si>
+  <si>
+    <t>Returns a Unit to the Hand</t>
+  </si>
+  <si>
+    <t>Arrow</t>
+  </si>
+  <si>
+    <t>Deal 3 Damage to a Unit</t>
+  </si>
+  <si>
+    <t>Warding Word</t>
+  </si>
+  <si>
+    <t>Give a Unit a protective Ward</t>
+  </si>
+  <si>
+    <t>Healing Whisper</t>
+  </si>
+  <si>
+    <t>Heal a Unit for 1 Health</t>
+  </si>
+  <si>
+    <t>Healing Shout</t>
+  </si>
+  <si>
+    <t>Heal a Unit for 2 Health</t>
+  </si>
+  <si>
+    <t>Buffet</t>
+  </si>
+  <si>
+    <t>Give a Unit 1 Overhealth</t>
+  </si>
+  <si>
+    <t>Sandvich</t>
+  </si>
+  <si>
+    <t>Give a Unit 2 Overhealth</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>Inspiring Aura (2), Grand Entrance</t>
+  </si>
+  <si>
+    <t>Commander</t>
+  </si>
+  <si>
+    <t>Petty Theif</t>
+  </si>
+  <si>
+    <t>Sneak Attack</t>
+  </si>
+  <si>
+    <t>Fleet Captain</t>
+  </si>
+  <si>
+    <t>Theif Boss</t>
+  </si>
+  <si>
+    <t>Assasain</t>
+  </si>
+  <si>
+    <t>Rightapult</t>
+  </si>
+  <si>
+    <t>Right Launcher</t>
+  </si>
+  <si>
+    <t>Leftapult</t>
+  </si>
+  <si>
+    <t>Left Launcher</t>
+  </si>
+  <si>
+    <t>Haybale</t>
+  </si>
+  <si>
+    <t>Immobile</t>
+  </si>
+  <si>
+    <t>Stone Barrier</t>
+  </si>
+  <si>
+    <t>Immobile, Shielding</t>
+  </si>
+  <si>
+    <t>Royal Guard</t>
+  </si>
+  <si>
+    <t>Inspiring Aura (1)</t>
+  </si>
+  <si>
+    <t>Druid Apprentice</t>
+  </si>
+  <si>
+    <t>Protective Aura (2)</t>
+  </si>
+  <si>
+    <t>Druid Master</t>
+  </si>
+  <si>
+    <t>Protective Aura (2), Healing Trail</t>
+  </si>
+  <si>
+    <t>Forest Spirit</t>
+  </si>
+  <si>
+    <t>Parting Gift</t>
+  </si>
+  <si>
+    <t>Goblin Demolitionist</t>
+  </si>
+  <si>
+    <t>Explosive Exit</t>
+  </si>
+  <si>
+    <t>Shielding, Braced (2)</t>
+  </si>
+  <si>
+    <t>Goblin Addict</t>
+  </si>
+  <si>
+    <t>Overtime, Last Laugh (2)</t>
+  </si>
+  <si>
+    <t>Lumberjack</t>
+  </si>
+  <si>
+    <t>Cleave</t>
+  </si>
+  <si>
+    <t>Grave Robber</t>
+  </si>
+  <si>
+    <t>Sneak Attack(2), Drive By (2)</t>
+  </si>
+  <si>
+    <t>Sneack Attack(3), Opportunistic(4)</t>
+  </si>
+  <si>
+    <t>Sneak Attack(1), Opportunistic(1)</t>
+  </si>
+  <si>
+    <t>Last Laugh (2)</t>
   </si>
 </sst>
 </file>
@@ -390,15 +624,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="149.140625" customWidth="1"/>
   </cols>
@@ -420,16 +654,406 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="colorScale" priority="3">
+  <autoFilter ref="A1:E4" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E24">
+      <sortCondition ref="B1:B4"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:B1048576">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <cfvo type="num" val="10"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -445,15 +1069,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="D2:D1048576">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <cfvo type="num" val="10"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -470,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72002C10-9D3D-4BE4-8EBB-15AA31D47463}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +1120,230 @@
       </c>
       <c r="D1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -523,10 +1371,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{513689B9-69CA-49E7-9489-7CE2039FD03C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8 B10:B1048576" xr:uid="{513689B9-69CA-49E7-9489-7CE2039FD03C}">
       <formula1>"Spell, Swift Spell"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{5BF3F793-7C8C-494C-8708-DC16C35A14E7}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C8 C10:C1048576" xr:uid="{5BF3F793-7C8C-494C-8708-DC16C35A14E7}">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Implemented Movement Traits, Placement Traits, & Status Effects
</commit_message>
<xml_diff>
--- a/doodle-deck-vault/cards.xlsx
+++ b/doodle-deck-vault/cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezb12\OneDrive\Desktop\doodle-deck\doodle-deck-vault\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA36B267-47E6-4DB3-87CE-6D8BA124816D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32962D8F-1070-42D2-A4D8-26D0A594FF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -181,21 +181,12 @@
     <t>Commander</t>
   </si>
   <si>
-    <t>Petty Theif</t>
-  </si>
-  <si>
     <t>Sneak Attack</t>
   </si>
   <si>
     <t>Fleet Captain</t>
   </si>
   <si>
-    <t>Theif Boss</t>
-  </si>
-  <si>
-    <t>Assasain</t>
-  </si>
-  <si>
     <t>Rightapult</t>
   </si>
   <si>
@@ -278,6 +269,15 @@
   </si>
   <si>
     <t>Last Laugh (2)</t>
+  </si>
+  <si>
+    <t>Petty Thief</t>
+  </si>
+  <si>
+    <t>Thief Boss</t>
+  </si>
+  <si>
+    <t>Assassin</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +670,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -682,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -704,7 +704,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -716,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -752,24 +752,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
         <v>50</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -781,12 +781,12 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -798,12 +798,12 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -815,12 +815,12 @@
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -832,12 +832,12 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -849,12 +849,12 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -866,29 +866,29 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
         <v>78</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -900,12 +900,12 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -917,12 +917,12 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -934,7 +934,7 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,12 +951,12 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -968,7 +968,7 @@
         <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -990,7 +990,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="B22">
         <v>7</v>
@@ -1002,7 +1002,7 @@
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B24">
         <v>7</v>
@@ -1036,7 +1036,7 @@
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1097,7 +1097,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>